<commit_message>
BackLog foi modificado com datas de entregas
</commit_message>
<xml_diff>
--- a/SmartPark-PI.xlsx
+++ b/SmartPark-PI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo Malan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo Malan\Desktop\Smart-Park\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{909F6404-F7B0-4D99-A30A-0F5D3BB08973}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517F67F7-E9BB-4439-9756-238FAEC691DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Classificação</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Arduino</t>
   </si>
   <si>
-    <t>Interface do layout do estacionamento</t>
-  </si>
-  <si>
     <t>R16</t>
   </si>
   <si>
@@ -173,7 +170,19 @@
     <t>Desejável</t>
   </si>
   <si>
-    <t>Pontuaçao</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Interface do layout do estacionamento (HLD/LLD)</t>
   </si>
 </sst>
 </file>
@@ -195,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,12 +214,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,17 +266,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -303,15 +309,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A2:F18" totalsRowShown="0">
-  <autoFilter ref="A2:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº do Requisito" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A2:I18" totalsRowShown="0">
+  <autoFilter ref="A2:I18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº do Requisito" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Requisito"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Classificação" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1B6BB76F-2BAA-41B4-A5FA-DD4283E659F7}" name="Tamanho" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8972AC04-1B98-447F-9558-5851A0E47202}" name="Sequência" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F26DA9DC-C5B4-4312-B530-28617757DCC0}" name="Pontuaçao" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Classificação" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1B6BB76F-2BAA-41B4-A5FA-DD4283E659F7}" name="Tamanho" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8972AC04-1B98-447F-9558-5851A0E47202}" name="Sequência" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E5CFF7D5-6A0E-44DF-83EF-B8331239DE6E}" name="1" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{74956A55-6EA5-4B14-A6AA-DBC0F9651002}" name="2" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{EBA4927F-CE55-4F35-B0AF-6E6CB6F7C0F7}" name="3" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{4F6CC372-4C81-45DE-AB7E-5A5C191DB01A}" name="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +602,9 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -607,35 +615,44 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
       <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="5">
         <v>13</v>
@@ -643,9 +660,14 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -653,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5">
         <v>21</v>
@@ -661,9 +683,14 @@
       <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -671,7 +698,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5">
         <v>8</v>
@@ -679,9 +706,14 @@
       <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -689,7 +721,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="5">
         <v>8</v>
@@ -697,9 +729,14 @@
       <c r="E6" s="5">
         <v>4</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -707,7 +744,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
@@ -715,14 +752,19 @@
       <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="G7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -733,9 +775,14 @@
       <c r="E8" s="5">
         <v>6</v>
       </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -743,7 +790,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5">
         <v>3</v>
@@ -751,9 +798,14 @@
       <c r="E9" s="5">
         <v>7</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -769,9 +821,14 @@
       <c r="E10" s="5">
         <v>8</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -779,7 +836,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="5">
         <v>5</v>
@@ -787,9 +844,14 @@
       <c r="E11" s="5">
         <v>9</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -797,7 +859,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5">
         <v>13</v>
@@ -805,11 +867,20 @@
       <c r="E12" s="5">
         <v>10</v>
       </c>
-      <c r="F12" s="11">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -822,48 +893,57 @@
       <c r="D13" s="8">
         <v>3</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>11</v>
       </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="8">
         <v>3</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>12</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="8">
         <v>3</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="6">
         <v>13</v>
       </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -876,48 +956,64 @@
       <c r="D16" s="8">
         <v>5</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="6">
         <v>14</v>
       </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>15</v>
       </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8">
         <v>13</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="6">
         <v>16</v>
       </c>
-      <c r="F18" s="11">
-        <v>112</v>
-      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>